<commit_message>
Nuevos tipos de material y tipos de tratamiento
</commit_message>
<xml_diff>
--- a/desarrollo/rigk-sg-back/files/templates/_carga_masiva_z.xlsx
+++ b/desarrollo/rigk-sg-back/files/templates/_carga_masiva_z.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="573">
   <si>
     <t>VAT</t>
   </si>
@@ -1286,6 +1286,9 @@
     <t>76860335-9</t>
   </si>
   <si>
+    <t>EMPRESA ZOR CI</t>
+  </si>
+  <si>
     <t>76933672-9</t>
   </si>
   <si>
@@ -1661,40 +1664,73 @@
     <t>PESO VALORIZADO</t>
   </si>
   <si>
-    <t>est_cm2 - Región de Arica y Parinacota</t>
+    <t>zor-ges-arica - Región de Arica y Parinacota</t>
   </si>
   <si>
     <t>Valorización Energética</t>
   </si>
   <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Envase Aluminio</t>
+  </si>
+  <si>
+    <t>11/09/2023</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>663</t>
+  </si>
+  <si>
+    <t>Disposición Final en RS</t>
+  </si>
+  <si>
+    <t>Plástico</t>
+  </si>
+  <si>
+    <t>Plástico Film Embalaje</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>662</t>
+  </si>
+  <si>
+    <t>Plástico Zuncho</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>664</t>
+  </si>
+  <si>
+    <t>zor-ges-santiago - Región Metropolitana</t>
+  </si>
+  <si>
+    <t>DF en Relleno Seguridad</t>
+  </si>
+  <si>
     <t>Madera</t>
   </si>
   <si>
     <t>Pallet de Madera</t>
   </si>
   <si>
-    <t>07/09/2023</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>656</t>
-  </si>
-  <si>
-    <t>Caja de Madera</t>
-  </si>
-  <si>
-    <t>08/09/2023</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>657</t>
+    <t>12/09/2023</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>666</t>
   </si>
 </sst>
 </file>
@@ -2723,8 +2759,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" name="_11992209_7" displayName="_11992209_7" ref="C1:C45" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="C1:C45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" name="_11992209_7" displayName="_11992209_7" ref="C1:C46" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="C1:C46">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
@@ -5336,569 +5372,572 @@
         <v>422</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>423</v>
       </c>
+      <c r="C46" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -6069,7 +6108,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
@@ -6089,136 +6128,224 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="F1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="G1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="I1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="J1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="K1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="L1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="M1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="G2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="H2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="I2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>554</v>
-      </c>
       <c r="N2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>373</v>
       </c>
       <c r="B3" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C3" t="s">
+        <v>558</v>
+      </c>
+      <c r="D3" t="s">
+        <v>559</v>
+      </c>
+      <c r="E3" t="s">
+        <v>560</v>
+      </c>
+      <c r="F3" t="s">
+        <v>554</v>
+      </c>
+      <c r="G3" t="s">
+        <v>555</v>
+      </c>
+      <c r="H3" t="s">
+        <v>555</v>
+      </c>
+      <c r="I3" t="s">
+        <v>555</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="N3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B4" t="s">
         <v>550</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>551</v>
       </c>
-      <c r="E3" t="s">
-        <v>557</v>
-      </c>
-      <c r="F3" t="s">
-        <v>558</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="D4" t="s">
+        <v>559</v>
+      </c>
+      <c r="E4" t="s">
+        <v>563</v>
+      </c>
+      <c r="F4" t="s">
         <v>554</v>
       </c>
-      <c r="H3" t="s">
-        <v>554</v>
-      </c>
-      <c r="I3" t="s">
-        <v>554</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="N3" t="s">
-        <v>560</v>
+      <c r="G4" t="s">
+        <v>555</v>
+      </c>
+      <c r="H4" t="s">
+        <v>555</v>
+      </c>
+      <c r="I4" t="s">
+        <v>555</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="N4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" t="s">
+        <v>567</v>
+      </c>
+      <c r="D5" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" t="s">
+        <v>569</v>
+      </c>
+      <c r="F5" t="s">
+        <v>570</v>
+      </c>
+      <c r="G5" t="s">
+        <v>555</v>
+      </c>
+      <c r="H5" t="s">
+        <v>555</v>
+      </c>
+      <c r="I5" t="s">
+        <v>555</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="N5" t="s">
+        <v>572</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" sqref="H2:H3">
+  <dataValidations count="6">
+    <dataValidation type="list" sqref="H2:H5">
       <formula1>Info!$A$2:$A$157</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="I2">
@@ -6227,7 +6354,13 @@
     <dataValidation type="list" sqref="I3">
       <formula1>=INDIRECT("_"&amp;SUBSTITUTE(H3,"-","_"))</formula1>
     </dataValidation>
-    <dataValidation type="textLength" showErrorMessage="1" errorStyle="error" errorTitle="Formato de Fecha Inválido" error="Por favor, ingrese una fecha válida en formato DD/MM/AAAA." sqref="J2:J3">
+    <dataValidation type="list" sqref="I4">
+      <formula1>=INDIRECT("_"&amp;SUBSTITUTE(H4,"-","_"))</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="I5">
+      <formula1>=INDIRECT("_"&amp;SUBSTITUTE(H5,"-","_"))</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" showErrorMessage="1" errorStyle="error" errorTitle="Formato de Fecha Inválido" error="Por favor, ingrese una fecha válida en formato DD/MM/AAAA." sqref="J2:J5">
       <formula1>10</formula1>
       <formula2>10</formula2>
     </dataValidation>

</xml_diff>